<commit_message>
Mise a jour du 11022026
Mise a jour du 11022026
</commit_message>
<xml_diff>
--- a/Listes_indicateurs_annuaire_stat.xlsx
+++ b/Listes_indicateurs_annuaire_stat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\monprojet1_annuaire\Production-statistique-MS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273B14A4-FF4E-4530-9A59-DAE767E39861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DBF626-478F-45D6-9A41-20D1FD26B265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3228" uniqueCount="2243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3260" uniqueCount="2267">
   <si>
     <t>listes_indicateurs</t>
   </si>
@@ -6770,6 +6770,78 @@
   </si>
   <si>
     <t>Obc-PVVIH ayant participé aux groupes de parole</t>
+  </si>
+  <si>
+    <t>Oh4nOTPDyYT</t>
+  </si>
+  <si>
+    <t>Activités d'IEC réalisées surTuberculose_Obc</t>
+  </si>
+  <si>
+    <t>SOzMaOoKYiV</t>
+  </si>
+  <si>
+    <t>Personnes touchées par les séances d'IEC sur la  Tuberculose_Obc</t>
+  </si>
+  <si>
+    <t>Obc-Personnes touchées par les séances d'IEC sur la  Tuberculose</t>
+  </si>
+  <si>
+    <t>Obc-Activités d'IEC réalisées surTuberculose_Obc</t>
+  </si>
+  <si>
+    <t>pA8xsQcCQJM</t>
+  </si>
+  <si>
+    <t>Personnes référées pour toux de plus de 14 jours_Obc</t>
+  </si>
+  <si>
+    <t>AJOagzS3KzW</t>
+  </si>
+  <si>
+    <t>Enfants de moins de 5 ans contact référés pour le dépistage_Obc</t>
+  </si>
+  <si>
+    <t>UAZK8g0We0T</t>
+  </si>
+  <si>
+    <t>Patients dépistés tuberculeux parmi les référés_Obc</t>
+  </si>
+  <si>
+    <t>ALY2wRceonY</t>
+  </si>
+  <si>
+    <t>Patients tuberculeux absents au traitement à rechercher_Obc</t>
+  </si>
+  <si>
+    <t>z5zDlTd1oIU</t>
+  </si>
+  <si>
+    <t>Patients tuberculeux absents au traitement retrouvés_Obc</t>
+  </si>
+  <si>
+    <t>u5XsrDgWoFj</t>
+  </si>
+  <si>
+    <t>Visites à domicile réalisées aux personnes_TB_Obc</t>
+  </si>
+  <si>
+    <t>Obc-Personnes référées pour toux de plus de 14 jours</t>
+  </si>
+  <si>
+    <t>Obc-Enfants de moins de 5 ans contact référés pour le dépistage</t>
+  </si>
+  <si>
+    <t>Obc-Patients dépistés tuberculeux parmi les référés</t>
+  </si>
+  <si>
+    <t>Obc-Patients tuberculeux absents au traitement à rechercher</t>
+  </si>
+  <si>
+    <t>Obc-Patients tuberculeux absents au traitement retrouvés</t>
+  </si>
+  <si>
+    <t>Obc-Visites à domicile réalisées aux personnes_TB</t>
   </si>
 </sst>
 </file>
@@ -6899,7 +6971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6929,9 +7001,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -7148,17 +7217,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z780"/>
+  <dimension ref="A1:Z782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A703" workbookViewId="0">
-      <selection activeCell="C715" sqref="C715"/>
+    <sheetView tabSelected="1" topLeftCell="A731" workbookViewId="0">
+      <selection activeCell="C745" sqref="C745"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="3" max="3" width="78.42578125" customWidth="1"/>
     <col min="4" max="4" width="54.7109375" customWidth="1"/>
     <col min="5" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="26" width="10.7109375" customWidth="1"/>
@@ -10660,13 +10729,13 @@
       <c r="A98" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B98" s="15" t="s">
+      <c r="B98" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="C98" s="14" t="s">
+      <c r="C98" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D98" s="14" t="s">
+      <c r="D98" s="1" t="s">
         <v>295</v>
       </c>
       <c r="E98" s="1"/>
@@ -32113,13 +32182,13 @@
       <c r="Z693" s="1"/>
     </row>
     <row r="694" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A694" s="14" t="s">
+      <c r="A694" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B694" s="1" t="s">
         <v>1986</v>
       </c>
-      <c r="C694" s="16" t="s">
+      <c r="C694" s="13" t="s">
         <v>1987</v>
       </c>
       <c r="D694" s="1" t="s">
@@ -32149,13 +32218,13 @@
       <c r="Z694" s="1"/>
     </row>
     <row r="695" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A695" s="14" t="s">
+      <c r="A695" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B695" s="1" t="s">
         <v>1988</v>
       </c>
-      <c r="C695" s="16" t="s">
+      <c r="C695" s="13" t="s">
         <v>1989</v>
       </c>
       <c r="D695" s="1" t="s">
@@ -32185,13 +32254,13 @@
       <c r="Z695" s="1"/>
     </row>
     <row r="696" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A696" s="14" t="s">
+      <c r="A696" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B696" s="1" t="s">
         <v>1990</v>
       </c>
-      <c r="C696" s="16" t="s">
+      <c r="C696" s="13" t="s">
         <v>1991</v>
       </c>
       <c r="D696" s="1" t="s">
@@ -32221,13 +32290,13 @@
       <c r="Z696" s="1"/>
     </row>
     <row r="697" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A697" s="14" t="s">
+      <c r="A697" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B697" s="1" t="s">
         <v>1992</v>
       </c>
-      <c r="C697" s="16" t="s">
+      <c r="C697" s="13" t="s">
         <v>1993</v>
       </c>
       <c r="D697" s="1" t="s">
@@ -32257,13 +32326,13 @@
       <c r="Z697" s="1"/>
     </row>
     <row r="698" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A698" s="14" t="s">
+      <c r="A698" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B698" s="1" t="s">
         <v>1994</v>
       </c>
-      <c r="C698" s="16" t="s">
+      <c r="C698" s="13" t="s">
         <v>1995</v>
       </c>
       <c r="D698" s="1" t="s">
@@ -32293,13 +32362,13 @@
       <c r="Z698" s="1"/>
     </row>
     <row r="699" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A699" s="14" t="s">
+      <c r="A699" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B699" s="1" t="s">
         <v>1996</v>
       </c>
-      <c r="C699" s="16" t="s">
+      <c r="C699" s="13" t="s">
         <v>1997</v>
       </c>
       <c r="D699" s="1" t="s">
@@ -32329,13 +32398,13 @@
       <c r="Z699" s="1"/>
     </row>
     <row r="700" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A700" s="14" t="s">
+      <c r="A700" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B700" s="1" t="s">
         <v>1998</v>
       </c>
-      <c r="C700" s="16" t="s">
+      <c r="C700" s="13" t="s">
         <v>1999</v>
       </c>
       <c r="D700" s="1" t="s">
@@ -32365,13 +32434,13 @@
       <c r="Z700" s="1"/>
     </row>
     <row r="701" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A701" s="14" t="s">
+      <c r="A701" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B701" s="1" t="s">
         <v>2000</v>
       </c>
-      <c r="C701" s="16" t="s">
+      <c r="C701" s="13" t="s">
         <v>2001</v>
       </c>
       <c r="D701" s="1" t="s">
@@ -32401,13 +32470,13 @@
       <c r="Z701" s="1"/>
     </row>
     <row r="702" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A702" s="14" t="s">
+      <c r="A702" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B702" s="1" t="s">
         <v>2002</v>
       </c>
-      <c r="C702" s="16" t="s">
+      <c r="C702" s="13" t="s">
         <v>2003</v>
       </c>
       <c r="D702" s="1" t="s">
@@ -32437,7 +32506,7 @@
       <c r="Z702" s="1"/>
     </row>
     <row r="703" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A703" s="14" t="s">
+      <c r="A703" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B703" s="1" t="s">
@@ -32473,7 +32542,7 @@
       <c r="Z703" s="1"/>
     </row>
     <row r="704" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A704" s="14" t="s">
+      <c r="A704" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B704" s="1" t="s">
@@ -32509,7 +32578,7 @@
       <c r="Z704" s="1"/>
     </row>
     <row r="705" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A705" s="14" t="s">
+      <c r="A705" s="1" t="s">
         <v>1985</v>
       </c>
       <c r="B705" s="1" t="s">
@@ -32545,7 +32614,7 @@
       <c r="Z705" s="1"/>
     </row>
     <row r="706" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A706" s="14" t="s">
+      <c r="A706" s="1" t="s">
         <v>2010</v>
       </c>
       <c r="B706" s="1" t="s">
@@ -32581,7 +32650,7 @@
       <c r="Z706" s="1"/>
     </row>
     <row r="707" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A707" s="14" t="s">
+      <c r="A707" s="1" t="s">
         <v>2010</v>
       </c>
       <c r="B707" s="1" t="s">
@@ -32617,7 +32686,7 @@
       <c r="Z707" s="1"/>
     </row>
     <row r="708" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A708" s="14" t="s">
+      <c r="A708" s="1" t="s">
         <v>2010</v>
       </c>
       <c r="B708" s="1" t="s">
@@ -32653,7 +32722,7 @@
       <c r="Z708" s="1"/>
     </row>
     <row r="709" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A709" s="13" t="s">
+      <c r="A709" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B709" s="12" t="s">
@@ -32688,7 +32757,7 @@
       <c r="Z709" s="1"/>
     </row>
     <row r="710" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A710" s="13" t="s">
+      <c r="A710" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B710" s="12" t="s">
@@ -32723,7 +32792,7 @@
       <c r="Z710" s="1"/>
     </row>
     <row r="711" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A711" s="13" t="s">
+      <c r="A711" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B711" s="12" t="s">
@@ -32758,7 +32827,7 @@
       <c r="Z711" s="1"/>
     </row>
     <row r="712" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A712" s="13" t="s">
+      <c r="A712" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B712" s="12" t="s">
@@ -32793,7 +32862,7 @@
       <c r="Z712" s="1"/>
     </row>
     <row r="713" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A713" s="13" t="s">
+      <c r="A713" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B713" s="12" t="s">
@@ -32828,7 +32897,7 @@
       <c r="Z713" s="1"/>
     </row>
     <row r="714" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A714" s="13" t="s">
+      <c r="A714" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B714" s="12" t="s">
@@ -32863,7 +32932,7 @@
       <c r="Z714" s="1"/>
     </row>
     <row r="715" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A715" s="13" t="s">
+      <c r="A715" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B715" s="12" t="s">
@@ -32898,17 +32967,17 @@
       <c r="Z715" s="1"/>
     </row>
     <row r="716" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A716" s="13" t="s">
+      <c r="A716" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B716" s="12" t="s">
-        <v>2191</v>
+        <v>2243</v>
       </c>
       <c r="C716" s="12" t="s">
-        <v>2192</v>
+        <v>2248</v>
       </c>
       <c r="D716" s="12" t="s">
-        <v>2192</v>
+        <v>2244</v>
       </c>
       <c r="F716" s="1"/>
       <c r="G716" s="1"/>
@@ -32933,17 +33002,17 @@
       <c r="Z716" s="1"/>
     </row>
     <row r="717" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A717" s="13" t="s">
+      <c r="A717" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B717" s="12" t="s">
-        <v>2193</v>
+        <v>2191</v>
       </c>
       <c r="C717" s="12" t="s">
-        <v>2194</v>
+        <v>2192</v>
       </c>
       <c r="D717" s="12" t="s">
-        <v>2194</v>
+        <v>2192</v>
       </c>
       <c r="F717" s="1"/>
       <c r="G717" s="1"/>
@@ -32968,17 +33037,17 @@
       <c r="Z717" s="1"/>
     </row>
     <row r="718" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A718" s="13" t="s">
+      <c r="A718" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B718" s="12" t="s">
-        <v>2195</v>
+        <v>2193</v>
       </c>
       <c r="C718" s="12" t="s">
-        <v>2196</v>
+        <v>2194</v>
       </c>
       <c r="D718" s="12" t="s">
-        <v>2196</v>
+        <v>2194</v>
       </c>
       <c r="F718" s="1"/>
       <c r="G718" s="1"/>
@@ -33003,17 +33072,17 @@
       <c r="Z718" s="1"/>
     </row>
     <row r="719" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A719" s="13" t="s">
+      <c r="A719" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B719" s="12" t="s">
-        <v>2197</v>
+        <v>2195</v>
       </c>
       <c r="C719" s="12" t="s">
-        <v>2198</v>
+        <v>2196</v>
       </c>
       <c r="D719" s="12" t="s">
-        <v>2198</v>
+        <v>2196</v>
       </c>
       <c r="F719" s="1"/>
       <c r="G719" s="1"/>
@@ -33038,17 +33107,17 @@
       <c r="Z719" s="1"/>
     </row>
     <row r="720" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A720" s="13" t="s">
+      <c r="A720" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B720" s="12" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
       <c r="C720" s="12" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="D720" s="12" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="F720" s="1"/>
       <c r="G720" s="1"/>
@@ -33073,17 +33142,17 @@
       <c r="Z720" s="1"/>
     </row>
     <row r="721" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A721" s="13" t="s">
+      <c r="A721" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B721" s="12" t="s">
-        <v>2201</v>
+        <v>2245</v>
       </c>
       <c r="C721" s="12" t="s">
-        <v>2202</v>
+        <v>2247</v>
       </c>
       <c r="D721" s="12" t="s">
-        <v>2202</v>
+        <v>2246</v>
       </c>
       <c r="F721" s="1"/>
       <c r="G721" s="1"/>
@@ -33108,17 +33177,17 @@
       <c r="Z721" s="1"/>
     </row>
     <row r="722" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A722" s="13" t="s">
+      <c r="A722" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B722" s="12" t="s">
-        <v>2203</v>
+        <v>2199</v>
       </c>
       <c r="C722" s="12" t="s">
-        <v>2204</v>
+        <v>2200</v>
       </c>
       <c r="D722" s="12" t="s">
-        <v>2204</v>
+        <v>2200</v>
       </c>
       <c r="F722" s="1"/>
       <c r="G722" s="1"/>
@@ -33143,17 +33212,17 @@
       <c r="Z722" s="1"/>
     </row>
     <row r="723" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A723" s="13" t="s">
+      <c r="A723" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B723" s="12" t="s">
-        <v>2205</v>
+        <v>2201</v>
       </c>
       <c r="C723" s="12" t="s">
-        <v>2241</v>
+        <v>2202</v>
       </c>
       <c r="D723" s="12" t="s">
-        <v>2206</v>
+        <v>2202</v>
       </c>
       <c r="F723" s="1"/>
       <c r="G723" s="1"/>
@@ -33178,17 +33247,17 @@
       <c r="Z723" s="1"/>
     </row>
     <row r="724" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A724" s="13" t="s">
+      <c r="A724" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B724" s="12" t="s">
-        <v>2207</v>
+        <v>2203</v>
       </c>
       <c r="C724" s="12" t="s">
-        <v>2242</v>
+        <v>2204</v>
       </c>
       <c r="D724" s="12" t="s">
-        <v>2208</v>
+        <v>2204</v>
       </c>
       <c r="F724" s="1"/>
       <c r="G724" s="1"/>
@@ -33213,17 +33282,17 @@
       <c r="Z724" s="1"/>
     </row>
     <row r="725" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A725" s="13" t="s">
+      <c r="A725" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B725" s="12" t="s">
-        <v>2209</v>
+        <v>2205</v>
       </c>
       <c r="C725" s="12" t="s">
-        <v>2210</v>
+        <v>2241</v>
       </c>
       <c r="D725" s="12" t="s">
-        <v>2210</v>
+        <v>2206</v>
       </c>
       <c r="F725" s="1"/>
       <c r="G725" s="1"/>
@@ -33248,17 +33317,17 @@
       <c r="Z725" s="1"/>
     </row>
     <row r="726" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A726" s="13" t="s">
+      <c r="A726" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B726" s="12" t="s">
-        <v>2211</v>
+        <v>2207</v>
       </c>
       <c r="C726" s="12" t="s">
-        <v>2212</v>
+        <v>2242</v>
       </c>
       <c r="D726" s="12" t="s">
-        <v>2212</v>
+        <v>2208</v>
       </c>
       <c r="F726" s="1"/>
       <c r="G726" s="1"/>
@@ -33283,17 +33352,17 @@
       <c r="Z726" s="1"/>
     </row>
     <row r="727" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A727" s="13" t="s">
+      <c r="A727" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B727" s="12" t="s">
-        <v>2213</v>
+        <v>2209</v>
       </c>
       <c r="C727" s="12" t="s">
-        <v>2214</v>
+        <v>2210</v>
       </c>
       <c r="D727" s="12" t="s">
-        <v>2214</v>
+        <v>2210</v>
       </c>
       <c r="F727" s="1"/>
       <c r="G727" s="1"/>
@@ -33318,17 +33387,17 @@
       <c r="Z727" s="1"/>
     </row>
     <row r="728" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A728" s="13" t="s">
+      <c r="A728" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B728" s="12" t="s">
-        <v>2215</v>
+        <v>2211</v>
       </c>
       <c r="C728" s="12" t="s">
-        <v>2216</v>
+        <v>2212</v>
       </c>
       <c r="D728" s="12" t="s">
-        <v>2216</v>
+        <v>2212</v>
       </c>
       <c r="F728" s="1"/>
       <c r="G728" s="1"/>
@@ -33353,17 +33422,17 @@
       <c r="Z728" s="1"/>
     </row>
     <row r="729" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A729" s="13" t="s">
+      <c r="A729" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B729" s="12" t="s">
-        <v>2217</v>
+        <v>2213</v>
       </c>
       <c r="C729" s="12" t="s">
-        <v>2218</v>
+        <v>2214</v>
       </c>
       <c r="D729" s="12" t="s">
-        <v>2218</v>
+        <v>2214</v>
       </c>
       <c r="F729" s="1"/>
       <c r="G729" s="1"/>
@@ -33388,17 +33457,17 @@
       <c r="Z729" s="1"/>
     </row>
     <row r="730" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A730" s="13" t="s">
+      <c r="A730" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B730" s="12" t="s">
-        <v>2219</v>
+        <v>2215</v>
       </c>
       <c r="C730" s="12" t="s">
-        <v>2220</v>
+        <v>2216</v>
       </c>
       <c r="D730" s="12" t="s">
-        <v>2220</v>
+        <v>2216</v>
       </c>
       <c r="F730" s="1"/>
       <c r="G730" s="1"/>
@@ -33423,17 +33492,17 @@
       <c r="Z730" s="1"/>
     </row>
     <row r="731" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A731" s="13" t="s">
+      <c r="A731" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B731" s="12" t="s">
-        <v>2221</v>
+        <v>2217</v>
       </c>
       <c r="C731" s="12" t="s">
-        <v>2222</v>
+        <v>2218</v>
       </c>
       <c r="D731" s="12" t="s">
-        <v>2222</v>
+        <v>2218</v>
       </c>
       <c r="F731" s="1"/>
       <c r="G731" s="1"/>
@@ -33458,7 +33527,7 @@
       <c r="Z731" s="1"/>
     </row>
     <row r="732" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A732" s="13" t="s">
+      <c r="A732" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B732" s="12" t="s">
@@ -33493,17 +33562,17 @@
       <c r="Z732" s="1"/>
     </row>
     <row r="733" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A733" s="13" t="s">
+      <c r="A733" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B733" s="12" t="s">
-        <v>2223</v>
+        <v>2221</v>
       </c>
       <c r="C733" s="12" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="D733" s="12" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="F733" s="1"/>
       <c r="G733" s="1"/>
@@ -33528,17 +33597,17 @@
       <c r="Z733" s="1"/>
     </row>
     <row r="734" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A734" s="13" t="s">
+      <c r="A734" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B734" s="12" t="s">
-        <v>2225</v>
+        <v>2219</v>
       </c>
       <c r="C734" s="12" t="s">
-        <v>2226</v>
+        <v>2220</v>
       </c>
       <c r="D734" s="12" t="s">
-        <v>2226</v>
+        <v>2220</v>
       </c>
       <c r="F734" s="1"/>
       <c r="G734" s="1"/>
@@ -33563,17 +33632,17 @@
       <c r="Z734" s="1"/>
     </row>
     <row r="735" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A735" s="13" t="s">
+      <c r="A735" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B735" s="12" t="s">
-        <v>2227</v>
+        <v>2223</v>
       </c>
       <c r="C735" s="12" t="s">
-        <v>2228</v>
+        <v>2224</v>
       </c>
       <c r="D735" s="12" t="s">
-        <v>2228</v>
+        <v>2224</v>
       </c>
       <c r="F735" s="1"/>
       <c r="G735" s="1"/>
@@ -33598,17 +33667,17 @@
       <c r="Z735" s="1"/>
     </row>
     <row r="736" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A736" s="13" t="s">
+      <c r="A736" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B736" s="12" t="s">
-        <v>2229</v>
+        <v>2225</v>
       </c>
       <c r="C736" s="12" t="s">
-        <v>2230</v>
+        <v>2226</v>
       </c>
       <c r="D736" s="12" t="s">
-        <v>2230</v>
+        <v>2226</v>
       </c>
       <c r="F736" s="1"/>
       <c r="G736" s="1"/>
@@ -33633,17 +33702,17 @@
       <c r="Z736" s="1"/>
     </row>
     <row r="737" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A737" s="13" t="s">
+      <c r="A737" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B737" s="12" t="s">
-        <v>2231</v>
+        <v>2227</v>
       </c>
       <c r="C737" s="12" t="s">
-        <v>2232</v>
+        <v>2228</v>
       </c>
       <c r="D737" s="12" t="s">
-        <v>2232</v>
+        <v>2228</v>
       </c>
       <c r="F737" s="1"/>
       <c r="G737" s="1"/>
@@ -33668,17 +33737,17 @@
       <c r="Z737" s="1"/>
     </row>
     <row r="738" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A738" s="13" t="s">
+      <c r="A738" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B738" s="12" t="s">
-        <v>2233</v>
+        <v>2229</v>
       </c>
       <c r="C738" s="12" t="s">
-        <v>2234</v>
+        <v>2230</v>
       </c>
       <c r="D738" s="12" t="s">
-        <v>2234</v>
+        <v>2230</v>
       </c>
       <c r="F738" s="1"/>
       <c r="G738" s="1"/>
@@ -33703,11 +33772,18 @@
       <c r="Z738" s="1"/>
     </row>
     <row r="739" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A739" s="1"/>
-      <c r="B739" s="1"/>
-      <c r="C739" s="1"/>
-      <c r="D739" s="1"/>
-      <c r="E739" s="1"/>
+      <c r="A739" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B739" s="12" t="s">
+        <v>2231</v>
+      </c>
+      <c r="C739" s="12" t="s">
+        <v>2232</v>
+      </c>
+      <c r="D739" s="12" t="s">
+        <v>2232</v>
+      </c>
       <c r="F739" s="1"/>
       <c r="G739" s="1"/>
       <c r="H739" s="1"/>
@@ -33731,11 +33807,18 @@
       <c r="Z739" s="1"/>
     </row>
     <row r="740" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A740" s="1"/>
-      <c r="B740" s="1"/>
-      <c r="C740" s="1"/>
-      <c r="D740" s="1"/>
-      <c r="E740" s="1"/>
+      <c r="A740" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B740" s="12" t="s">
+        <v>2233</v>
+      </c>
+      <c r="C740" s="12" t="s">
+        <v>2234</v>
+      </c>
+      <c r="D740" s="12" t="s">
+        <v>2234</v>
+      </c>
       <c r="F740" s="1"/>
       <c r="G740" s="1"/>
       <c r="H740" s="1"/>
@@ -33759,10 +33842,18 @@
       <c r="Z740" s="1"/>
     </row>
     <row r="741" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A741" s="1"/>
-      <c r="B741" s="1"/>
-      <c r="C741" s="1"/>
-      <c r="D741" s="1"/>
+      <c r="A741" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B741" s="1" t="s">
+        <v>2249</v>
+      </c>
+      <c r="C741" s="1" t="s">
+        <v>2261</v>
+      </c>
+      <c r="D741" s="1" t="s">
+        <v>2250</v>
+      </c>
       <c r="E741" s="1"/>
       <c r="F741" s="1"/>
       <c r="G741" s="1"/>
@@ -33787,10 +33878,18 @@
       <c r="Z741" s="1"/>
     </row>
     <row r="742" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A742" s="1"/>
-      <c r="B742" s="1"/>
-      <c r="C742" s="1"/>
-      <c r="D742" s="1"/>
+      <c r="A742" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B742" s="1" t="s">
+        <v>2251</v>
+      </c>
+      <c r="C742" s="1" t="s">
+        <v>2262</v>
+      </c>
+      <c r="D742" s="1" t="s">
+        <v>2252</v>
+      </c>
       <c r="E742" s="1"/>
       <c r="F742" s="1"/>
       <c r="G742" s="1"/>
@@ -33815,10 +33914,18 @@
       <c r="Z742" s="1"/>
     </row>
     <row r="743" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A743" s="1"/>
-      <c r="B743" s="1"/>
-      <c r="C743" s="1"/>
-      <c r="D743" s="1"/>
+      <c r="A743" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B743" s="1" t="s">
+        <v>2253</v>
+      </c>
+      <c r="C743" s="1" t="s">
+        <v>2263</v>
+      </c>
+      <c r="D743" s="1" t="s">
+        <v>2254</v>
+      </c>
       <c r="E743" s="1"/>
       <c r="F743" s="1"/>
       <c r="G743" s="1"/>
@@ -33843,10 +33950,18 @@
       <c r="Z743" s="1"/>
     </row>
     <row r="744" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A744" s="1"/>
-      <c r="B744" s="1"/>
-      <c r="C744" s="1"/>
-      <c r="D744" s="1"/>
+      <c r="A744" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B744" s="1" t="s">
+        <v>2255</v>
+      </c>
+      <c r="C744" s="1" t="s">
+        <v>2264</v>
+      </c>
+      <c r="D744" s="1" t="s">
+        <v>2256</v>
+      </c>
       <c r="E744" s="1"/>
       <c r="F744" s="1"/>
       <c r="G744" s="1"/>
@@ -33871,10 +33986,18 @@
       <c r="Z744" s="1"/>
     </row>
     <row r="745" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A745" s="1"/>
-      <c r="B745" s="1"/>
-      <c r="C745" s="1"/>
-      <c r="D745" s="1"/>
+      <c r="A745" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B745" s="1" t="s">
+        <v>2257</v>
+      </c>
+      <c r="C745" s="1" t="s">
+        <v>2265</v>
+      </c>
+      <c r="D745" s="1" t="s">
+        <v>2258</v>
+      </c>
       <c r="E745" s="1"/>
       <c r="F745" s="1"/>
       <c r="G745" s="1"/>
@@ -33899,10 +34022,18 @@
       <c r="Z745" s="1"/>
     </row>
     <row r="746" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A746" s="1"/>
-      <c r="B746" s="1"/>
-      <c r="C746" s="1"/>
-      <c r="D746" s="1"/>
+      <c r="A746" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B746" s="1" t="s">
+        <v>2259</v>
+      </c>
+      <c r="C746" s="1" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D746" s="1" t="s">
+        <v>2260</v>
+      </c>
       <c r="E746" s="1"/>
       <c r="F746" s="1"/>
       <c r="G746" s="1"/>
@@ -34878,6 +35009,62 @@
       <c r="Y780" s="1"/>
       <c r="Z780" s="1"/>
     </row>
+    <row r="781" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A781" s="1"/>
+      <c r="B781" s="1"/>
+      <c r="C781" s="1"/>
+      <c r="D781" s="1"/>
+      <c r="E781" s="1"/>
+      <c r="F781" s="1"/>
+      <c r="G781" s="1"/>
+      <c r="H781" s="1"/>
+      <c r="I781" s="1"/>
+      <c r="J781" s="1"/>
+      <c r="K781" s="1"/>
+      <c r="L781" s="1"/>
+      <c r="M781" s="1"/>
+      <c r="N781" s="1"/>
+      <c r="O781" s="1"/>
+      <c r="P781" s="1"/>
+      <c r="Q781" s="1"/>
+      <c r="R781" s="1"/>
+      <c r="S781" s="1"/>
+      <c r="T781" s="1"/>
+      <c r="U781" s="1"/>
+      <c r="V781" s="1"/>
+      <c r="W781" s="1"/>
+      <c r="X781" s="1"/>
+      <c r="Y781" s="1"/>
+      <c r="Z781" s="1"/>
+    </row>
+    <row r="782" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A782" s="1"/>
+      <c r="B782" s="1"/>
+      <c r="C782" s="1"/>
+      <c r="D782" s="1"/>
+      <c r="E782" s="1"/>
+      <c r="F782" s="1"/>
+      <c r="G782" s="1"/>
+      <c r="H782" s="1"/>
+      <c r="I782" s="1"/>
+      <c r="J782" s="1"/>
+      <c r="K782" s="1"/>
+      <c r="L782" s="1"/>
+      <c r="M782" s="1"/>
+      <c r="N782" s="1"/>
+      <c r="O782" s="1"/>
+      <c r="P782" s="1"/>
+      <c r="Q782" s="1"/>
+      <c r="R782" s="1"/>
+      <c r="S782" s="1"/>
+      <c r="T782" s="1"/>
+      <c r="U782" s="1"/>
+      <c r="V782" s="1"/>
+      <c r="W782" s="1"/>
+      <c r="X782" s="1"/>
+      <c r="Y782" s="1"/>
+      <c r="Z782" s="1"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>